<commit_message>
Feat: Enhance agent functionality by integrating Strategist and updating workflow
- Added Strategist component to AgentFactory for improved decision-making.
- Updated Workflow to include a new node for the Strategist and conditional edges.
- Modified Nodes class to handle team data and integrate with the new Strategist functionality.
- Updated QueryAnalyzer to process a list of teams alongside user queries.
- Enhanced state management to include a list of teams for better context in responses.
- Added new prompts for the Strategist to facilitate detailed analyses and predictions.
</commit_message>
<xml_diff>
--- a/Teams/Arsenal_stats.xlsx
+++ b/Teams/Arsenal_stats.xlsx
@@ -8,15 +8,15 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Matches" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="StandardStats" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ShootingStats" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PassingStats" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PassTypes" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GoalShotCreation" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DefensiveActions" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Standard Stats" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Shooting Stats" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Passing Stats" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pass Types" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Goal &amp; Shot Creation" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Defensive Actions" sheetId="7" state="visible" r:id="rId7"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Possession" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PlayingTime" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MiscStats" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Playing Time" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Miscellaneous Stats" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -5596,7 +5596,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>29-186</t>
+          <t>29-187</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -5677,7 +5677,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>23-361</t>
+          <t>23-362</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -5758,7 +5758,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>27-091</t>
+          <t>27-092</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -5839,7 +5839,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>23-276</t>
+          <t>23-277</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -5920,7 +5920,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>26-065</t>
+          <t>26-066</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -6001,7 +6001,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>31-280</t>
+          <t>31-281</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -6082,7 +6082,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>30-106</t>
+          <t>30-107</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -6163,7 +6163,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>25-282</t>
+          <t>25-283</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -6244,7 +6244,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>26-093</t>
+          <t>26-094</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -6325,7 +6325,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>23-275</t>
+          <t>23-276</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -6406,7 +6406,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>23-196</t>
+          <t>23-197</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -6487,7 +6487,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>28-271</t>
+          <t>28-272</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -6568,7 +6568,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>22-305</t>
+          <t>22-306</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -6649,7 +6649,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>18-175</t>
+          <t>18-176</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -6730,7 +6730,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>27-163</t>
+          <t>27-164</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -6811,7 +6811,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>17-364</t>
+          <t>18-000</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -6892,7 +6892,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>33-090</t>
+          <t>33-091</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -6973,7 +6973,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>27-351</t>
+          <t>27-352</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -7054,7 +7054,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>30-102</t>
+          <t>30-103</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -7135,7 +7135,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>25-033</t>
+          <t>25-034</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -7216,7 +7216,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>28-095</t>
+          <t>28-096</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -7297,7 +7297,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>27-288</t>
+          <t>27-289</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -7378,7 +7378,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>26-135</t>
+          <t>26-136</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -7457,7 +7457,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>25-100</t>
+          <t>25-101</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -7947,7 +7947,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>29-186</t>
+          <t>29-187</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -8064,7 +8064,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>23-361</t>
+          <t>23-362</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -8181,7 +8181,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>27-091</t>
+          <t>27-092</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -8298,7 +8298,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>23-276</t>
+          <t>23-277</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -8415,7 +8415,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>26-065</t>
+          <t>26-066</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -8532,7 +8532,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>31-280</t>
+          <t>31-281</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -8649,7 +8649,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>30-106</t>
+          <t>30-107</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -8766,7 +8766,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>25-282</t>
+          <t>25-283</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -8883,7 +8883,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>26-093</t>
+          <t>26-094</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -9000,7 +9000,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>23-275</t>
+          <t>23-276</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -9117,7 +9117,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>23-196</t>
+          <t>23-197</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -9234,7 +9234,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>28-271</t>
+          <t>28-272</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -9351,7 +9351,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>22-305</t>
+          <t>22-306</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -9468,7 +9468,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>18-175</t>
+          <t>18-176</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -9585,7 +9585,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>27-163</t>
+          <t>27-164</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -9702,7 +9702,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>17-364</t>
+          <t>18-000</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -9819,7 +9819,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>33-090</t>
+          <t>33-091</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -9936,7 +9936,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>27-351</t>
+          <t>27-352</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -10053,7 +10053,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>30-102</t>
+          <t>30-103</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -10170,7 +10170,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>25-033</t>
+          <t>25-034</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -10287,7 +10287,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>28-095</t>
+          <t>28-096</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -10404,7 +10404,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>27-288</t>
+          <t>27-289</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -10521,7 +10521,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>26-135</t>
+          <t>26-136</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -10638,7 +10638,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>25-100</t>
+          <t>25-101</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -10755,7 +10755,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>22-075</t>
+          <t>22-076</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -10818,7 +10818,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>18-179</t>
+          <t>18-180</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -10881,7 +10881,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>19-100</t>
+          <t>19-101</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -10944,7 +10944,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>19-167</t>
+          <t>19-168</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -11007,7 +11007,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>35-244</t>
+          <t>35-245</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -11070,7 +11070,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>18-237</t>
+          <t>18-238</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -11133,7 +11133,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>25-294</t>
+          <t>25-295</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -11196,7 +11196,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>21-212</t>
+          <t>21-213</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -11259,7 +11259,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>16-248</t>
+          <t>16-249</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -11322,7 +11322,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>26-310</t>
+          <t>26-311</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -11385,7 +11385,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>19-007</t>
+          <t>19-008</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -11860,7 +11860,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>29-186</t>
+          <t>29-187</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -11934,7 +11934,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>23-361</t>
+          <t>23-362</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -12018,7 +12018,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>27-091</t>
+          <t>27-092</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -12102,7 +12102,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>23-276</t>
+          <t>23-277</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -12186,7 +12186,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>26-065</t>
+          <t>26-066</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -12270,7 +12270,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>31-280</t>
+          <t>31-281</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -12354,7 +12354,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>30-106</t>
+          <t>30-107</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -12438,7 +12438,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>25-282</t>
+          <t>25-283</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -12522,7 +12522,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>26-093</t>
+          <t>26-094</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -12606,7 +12606,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>23-275</t>
+          <t>23-276</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -12690,7 +12690,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>23-196</t>
+          <t>23-197</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -12774,7 +12774,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>28-271</t>
+          <t>28-272</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -12858,7 +12858,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>22-305</t>
+          <t>22-306</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -12942,7 +12942,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>18-175</t>
+          <t>18-176</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -13026,7 +13026,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>27-163</t>
+          <t>27-164</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -13110,7 +13110,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>17-364</t>
+          <t>18-000</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -13194,7 +13194,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>33-090</t>
+          <t>33-091</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -13276,7 +13276,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>27-351</t>
+          <t>27-352</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -13360,7 +13360,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>30-102</t>
+          <t>30-103</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -13442,7 +13442,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>25-033</t>
+          <t>25-034</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -13516,7 +13516,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>28-095</t>
+          <t>28-096</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -13598,7 +13598,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>27-288</t>
+          <t>27-289</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -13680,7 +13680,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>26-135</t>
+          <t>26-136</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -13762,7 +13762,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>25-100</t>
+          <t>25-101</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -14255,7 +14255,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>29-186</t>
+          <t>29-187</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -14357,7 +14357,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>23-361</t>
+          <t>23-362</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -14459,7 +14459,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>27-091</t>
+          <t>27-092</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -14561,7 +14561,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>23-276</t>
+          <t>23-277</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -14663,7 +14663,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>26-065</t>
+          <t>26-066</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -14765,7 +14765,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>31-280</t>
+          <t>31-281</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -14867,7 +14867,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>30-106</t>
+          <t>30-107</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -14969,7 +14969,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>25-282</t>
+          <t>25-283</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -15071,7 +15071,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>26-093</t>
+          <t>26-094</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -15173,7 +15173,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>23-275</t>
+          <t>23-276</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -15275,7 +15275,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>23-196</t>
+          <t>23-197</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -15377,7 +15377,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>28-271</t>
+          <t>28-272</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -15479,7 +15479,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>22-305</t>
+          <t>22-306</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -15581,7 +15581,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>18-175</t>
+          <t>18-176</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -15683,7 +15683,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>27-163</t>
+          <t>27-164</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -15785,7 +15785,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>17-364</t>
+          <t>18-000</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -15887,7 +15887,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>33-090</t>
+          <t>33-091</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -15989,7 +15989,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>27-351</t>
+          <t>27-352</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -16091,7 +16091,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>30-102</t>
+          <t>30-103</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -16193,7 +16193,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>25-033</t>
+          <t>25-034</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -16295,7 +16295,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>28-095</t>
+          <t>28-096</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -16397,7 +16397,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>27-288</t>
+          <t>27-289</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -16499,7 +16499,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>26-135</t>
+          <t>26-136</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -16601,7 +16601,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>25-100</t>
+          <t>25-101</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -17073,7 +17073,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>29-186</t>
+          <t>29-187</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -17151,7 +17151,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>23-361</t>
+          <t>23-362</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -17229,7 +17229,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>27-091</t>
+          <t>27-092</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -17307,7 +17307,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>23-276</t>
+          <t>23-277</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -17385,7 +17385,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>26-065</t>
+          <t>26-066</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -17463,7 +17463,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>31-280</t>
+          <t>31-281</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -17541,7 +17541,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>30-106</t>
+          <t>30-107</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -17619,7 +17619,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>25-282</t>
+          <t>25-283</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -17697,7 +17697,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>26-093</t>
+          <t>26-094</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -17775,7 +17775,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>23-275</t>
+          <t>23-276</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -17853,7 +17853,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>23-196</t>
+          <t>23-197</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -17931,7 +17931,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>28-271</t>
+          <t>28-272</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -18009,7 +18009,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>22-305</t>
+          <t>22-306</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -18087,7 +18087,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>18-175</t>
+          <t>18-176</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -18165,7 +18165,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>27-163</t>
+          <t>27-164</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -18243,7 +18243,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>17-364</t>
+          <t>18-000</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -18321,7 +18321,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>33-090</t>
+          <t>33-091</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -18399,7 +18399,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>27-351</t>
+          <t>27-352</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -18477,7 +18477,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>30-102</t>
+          <t>30-103</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -18555,7 +18555,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>25-033</t>
+          <t>25-034</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -18633,7 +18633,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>28-095</t>
+          <t>28-096</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -18711,7 +18711,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>27-288</t>
+          <t>27-289</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -18789,7 +18789,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>26-135</t>
+          <t>26-136</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -18867,7 +18867,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>25-100</t>
+          <t>25-101</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -19279,7 +19279,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>29-186</t>
+          <t>29-187</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -19360,7 +19360,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>23-361</t>
+          <t>23-362</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -19441,7 +19441,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>27-091</t>
+          <t>27-092</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -19522,7 +19522,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>23-276</t>
+          <t>23-277</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -19603,7 +19603,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>26-065</t>
+          <t>26-066</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -19684,7 +19684,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>31-280</t>
+          <t>31-281</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -19765,7 +19765,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>30-106</t>
+          <t>30-107</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -19846,7 +19846,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>25-282</t>
+          <t>25-283</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -19927,7 +19927,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>26-093</t>
+          <t>26-094</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -20008,7 +20008,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>23-275</t>
+          <t>23-276</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -20089,7 +20089,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>23-196</t>
+          <t>23-197</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -20170,7 +20170,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>28-271</t>
+          <t>28-272</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -20251,7 +20251,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>22-305</t>
+          <t>22-306</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -20332,7 +20332,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>18-175</t>
+          <t>18-176</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -20413,7 +20413,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>27-163</t>
+          <t>27-164</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -20494,7 +20494,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>17-364</t>
+          <t>18-000</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -20575,7 +20575,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>33-090</t>
+          <t>33-091</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -20656,7 +20656,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>27-351</t>
+          <t>27-352</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -20737,7 +20737,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>30-102</t>
+          <t>30-103</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -20818,7 +20818,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>25-033</t>
+          <t>25-034</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -20899,7 +20899,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>28-095</t>
+          <t>28-096</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -20980,7 +20980,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>27-288</t>
+          <t>27-289</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -21061,7 +21061,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>26-135</t>
+          <t>26-136</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -21142,7 +21142,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>25-100</t>
+          <t>25-101</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -21576,7 +21576,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>29-186</t>
+          <t>29-187</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -21657,7 +21657,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>23-361</t>
+          <t>23-362</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -21738,7 +21738,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>27-091</t>
+          <t>27-092</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -21819,7 +21819,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>23-276</t>
+          <t>23-277</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -21900,7 +21900,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>26-065</t>
+          <t>26-066</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -21981,7 +21981,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>31-280</t>
+          <t>31-281</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -22062,7 +22062,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>30-106</t>
+          <t>30-107</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -22143,7 +22143,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>25-282</t>
+          <t>25-283</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -22224,7 +22224,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>26-093</t>
+          <t>26-094</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -22305,7 +22305,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>23-275</t>
+          <t>23-276</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -22386,7 +22386,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>23-196</t>
+          <t>23-197</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -22467,7 +22467,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>28-271</t>
+          <t>28-272</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -22548,7 +22548,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>22-305</t>
+          <t>22-306</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -22629,7 +22629,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>18-175</t>
+          <t>18-176</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -22710,7 +22710,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>27-163</t>
+          <t>27-164</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -22791,7 +22791,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>17-364</t>
+          <t>18-000</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -22872,7 +22872,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>33-090</t>
+          <t>33-091</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -22953,7 +22953,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>27-351</t>
+          <t>27-352</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -23034,7 +23034,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>30-102</t>
+          <t>30-103</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -23115,7 +23115,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>25-033</t>
+          <t>25-034</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -23196,7 +23196,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>28-095</t>
+          <t>28-096</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -23277,7 +23277,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>27-288</t>
+          <t>27-289</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -23358,7 +23358,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>26-135</t>
+          <t>26-136</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -23437,7 +23437,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>25-100</t>
+          <t>25-101</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -23894,7 +23894,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>29-186</t>
+          <t>29-187</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -23993,7 +23993,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>23-361</t>
+          <t>23-362</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -24092,7 +24092,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>27-091</t>
+          <t>27-092</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -24191,7 +24191,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>23-276</t>
+          <t>23-277</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -24290,7 +24290,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>26-065</t>
+          <t>26-066</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -24389,7 +24389,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>31-280</t>
+          <t>31-281</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -24488,7 +24488,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>30-106</t>
+          <t>30-107</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -24587,7 +24587,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>25-282</t>
+          <t>25-283</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -24686,7 +24686,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>26-093</t>
+          <t>26-094</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -24785,7 +24785,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>23-275</t>
+          <t>23-276</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -24884,7 +24884,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>23-196</t>
+          <t>23-197</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -24983,7 +24983,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>28-271</t>
+          <t>28-272</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -25082,7 +25082,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>22-305</t>
+          <t>22-306</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -25181,7 +25181,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>18-175</t>
+          <t>18-176</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -25280,7 +25280,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>27-163</t>
+          <t>27-164</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -25379,7 +25379,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>17-364</t>
+          <t>18-000</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -25478,7 +25478,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>33-090</t>
+          <t>33-091</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -25577,7 +25577,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>27-351</t>
+          <t>27-352</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -25676,7 +25676,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>30-102</t>
+          <t>30-103</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -25775,7 +25775,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>25-033</t>
+          <t>25-034</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -25874,7 +25874,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>28-095</t>
+          <t>28-096</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -25973,7 +25973,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>27-288</t>
+          <t>27-289</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -26072,7 +26072,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>26-135</t>
+          <t>26-136</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -26167,7 +26167,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>25-100</t>
+          <t>25-101</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -26711,7 +26711,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>29-186</t>
+          <t>29-187</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -26828,7 +26828,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>23-361</t>
+          <t>23-362</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -26945,7 +26945,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>27-091</t>
+          <t>27-092</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -27062,7 +27062,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>23-276</t>
+          <t>23-277</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -27179,7 +27179,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>26-065</t>
+          <t>26-066</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -27296,7 +27296,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>31-280</t>
+          <t>31-281</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -27413,7 +27413,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>30-106</t>
+          <t>30-107</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -27530,7 +27530,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>25-282</t>
+          <t>25-283</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -27647,7 +27647,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>26-093</t>
+          <t>26-094</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -27764,7 +27764,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>23-275</t>
+          <t>23-276</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -27881,7 +27881,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>23-196</t>
+          <t>23-197</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -27998,7 +27998,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>28-271</t>
+          <t>28-272</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -28115,7 +28115,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>22-305</t>
+          <t>22-306</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -28232,7 +28232,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>18-175</t>
+          <t>18-176</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -28349,7 +28349,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>27-163</t>
+          <t>27-164</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -28466,7 +28466,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>17-364</t>
+          <t>18-000</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -28583,7 +28583,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>33-090</t>
+          <t>33-091</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -28700,7 +28700,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>27-351</t>
+          <t>27-352</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -28817,7 +28817,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>30-102</t>
+          <t>30-103</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -28934,7 +28934,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>25-033</t>
+          <t>25-034</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -29051,7 +29051,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>28-095</t>
+          <t>28-096</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -29168,7 +29168,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>27-288</t>
+          <t>27-289</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -29285,7 +29285,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>26-135</t>
+          <t>26-136</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -29402,7 +29402,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>25-100</t>
+          <t>25-101</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -29519,7 +29519,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>22-075</t>
+          <t>22-076</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -29582,7 +29582,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>18-179</t>
+          <t>18-180</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -29645,7 +29645,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>19-100</t>
+          <t>19-101</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -29708,7 +29708,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>19-167</t>
+          <t>19-168</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -29771,7 +29771,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>35-244</t>
+          <t>35-245</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -29834,7 +29834,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>18-237</t>
+          <t>18-238</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -29897,7 +29897,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>25-294</t>
+          <t>25-295</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -29960,7 +29960,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>21-212</t>
+          <t>21-213</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -30023,7 +30023,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>16-248</t>
+          <t>16-249</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -30086,7 +30086,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>26-310</t>
+          <t>26-311</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -30149,7 +30149,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>19-007</t>
+          <t>19-008</t>
         </is>
       </c>
       <c r="F38" t="n">

</xml_diff>

<commit_message>
Feat: Enhance data handling, Add system initialization and integrate new functionalities for football analysis
What?
- Added initialization for the betting system
- Updated AgentFactory to include RAG data for the Strategist component.
- Introduced a new script for testing Chroma retrieval results.
- Refactoring
    1. Revised frontend to utilize Workflow for fetching responses.
    2. Revised RAG for a better integration with busuiness logic
- Added new methods in Workflow for improved response handling.
- Created markdown files for various teams' statistics and updated existing data structures.
- Established a Chroma database for efficient data storage and RAG retrieval.
</commit_message>
<xml_diff>
--- a/Teams/Arsenal_stats.xlsx
+++ b/Teams/Arsenal_stats.xlsx
@@ -7,16 +7,16 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Matches" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Standard Stats" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Shooting Stats" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Passing Stats" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pass Types" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Goal &amp; Shot Creation" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Defensive Actions" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Possession" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Playing Time" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Miscellaneous Stats" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Standard Stats" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Shooting Stats" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Passing Stats" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pass Types" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Goal &amp; Shot Creation" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Defensive Actions" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Possession" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Playing Time" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Miscellaneous Stats" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet_9" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4582,7 +4582,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>17:30</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -4940,7 +4940,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>29-190</t>
+          <t>29-193</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -5011,7 +5011,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>24-000</t>
+          <t>24-003</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -5082,7 +5082,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>27-095</t>
+          <t>27-098</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -5153,7 +5153,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>23-280</t>
+          <t>23-283</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -5224,7 +5224,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>26-069</t>
+          <t>26-072</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -5295,7 +5295,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>31-284</t>
+          <t>31-287</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -5366,7 +5366,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>30-110</t>
+          <t>30-113</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -5437,7 +5437,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>25-286</t>
+          <t>25-289</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -5508,7 +5508,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>26-097</t>
+          <t>26-100</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -5579,7 +5579,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>23-279</t>
+          <t>23-282</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -5650,7 +5650,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>23-200</t>
+          <t>23-203</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -5721,7 +5721,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>28-275</t>
+          <t>28-278</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -5792,7 +5792,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>22-309</t>
+          <t>22-312</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -5863,7 +5863,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>18-179</t>
+          <t>18-182</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -5934,7 +5934,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>27-167</t>
+          <t>27-170</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -6005,7 +6005,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>18-003</t>
+          <t>18-006</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -6076,7 +6076,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>33-094</t>
+          <t>33-097</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -6147,7 +6147,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>27-355</t>
+          <t>27-358</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -6218,7 +6218,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>30-106</t>
+          <t>30-109</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -6289,7 +6289,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>25-037</t>
+          <t>25-040</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -6360,7 +6360,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>28-099</t>
+          <t>28-102</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -6431,7 +6431,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>27-292</t>
+          <t>27-295</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -6502,7 +6502,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>26-139</t>
+          <t>26-142</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -6571,7 +6571,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>25-104</t>
+          <t>25-107</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -7016,7 +7016,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>29-190</t>
+          <t>29-193</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -7123,7 +7123,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>24-000</t>
+          <t>24-003</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -7230,7 +7230,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>27-095</t>
+          <t>27-098</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -7337,7 +7337,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>23-280</t>
+          <t>23-283</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -7444,7 +7444,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>26-069</t>
+          <t>26-072</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -7551,7 +7551,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>31-284</t>
+          <t>31-287</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -7658,7 +7658,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>30-110</t>
+          <t>30-113</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -7765,7 +7765,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>25-286</t>
+          <t>25-289</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -7872,7 +7872,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>26-097</t>
+          <t>26-100</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -7979,7 +7979,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>23-279</t>
+          <t>23-282</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -8086,7 +8086,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>23-200</t>
+          <t>23-203</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -8193,7 +8193,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>28-275</t>
+          <t>28-278</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -8300,7 +8300,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>22-309</t>
+          <t>22-312</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -8407,7 +8407,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>18-179</t>
+          <t>18-182</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -8514,7 +8514,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>27-167</t>
+          <t>27-170</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -8621,7 +8621,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>18-003</t>
+          <t>18-006</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -8728,7 +8728,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>33-094</t>
+          <t>33-097</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -8835,7 +8835,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>27-355</t>
+          <t>27-358</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -8942,7 +8942,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>30-106</t>
+          <t>30-109</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -9049,7 +9049,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>25-037</t>
+          <t>25-040</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -9156,7 +9156,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>28-099</t>
+          <t>28-102</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -9263,7 +9263,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>27-292</t>
+          <t>27-295</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -9370,7 +9370,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>26-139</t>
+          <t>26-142</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -9477,7 +9477,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>25-104</t>
+          <t>25-107</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -9584,7 +9584,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>22-079</t>
+          <t>22-082</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -9637,7 +9637,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>18-183</t>
+          <t>18-186</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -9690,7 +9690,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>19-104</t>
+          <t>19-107</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -9743,7 +9743,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>19-171</t>
+          <t>19-174</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -9796,7 +9796,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>35-248</t>
+          <t>35-251</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -9849,7 +9849,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>18-241</t>
+          <t>18-244</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -9902,7 +9902,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>25-298</t>
+          <t>25-301</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -9955,7 +9955,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>21-216</t>
+          <t>21-219</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -10008,7 +10008,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>16-252</t>
+          <t>16-255</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -10061,7 +10061,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>26-314</t>
+          <t>26-317</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -10114,7 +10114,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>19-011</t>
+          <t>19-014</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -10540,7 +10540,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>29-190</t>
+          <t>29-193</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -10604,7 +10604,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>24-000</t>
+          <t>24-003</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -10678,7 +10678,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>27-095</t>
+          <t>27-098</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -10752,7 +10752,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>23-280</t>
+          <t>23-283</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -10826,7 +10826,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>26-069</t>
+          <t>26-072</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -10900,7 +10900,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>31-284</t>
+          <t>31-287</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -10974,7 +10974,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>30-110</t>
+          <t>30-113</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -11048,7 +11048,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>25-286</t>
+          <t>25-289</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -11122,7 +11122,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>26-097</t>
+          <t>26-100</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -11196,7 +11196,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>23-279</t>
+          <t>23-282</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -11270,7 +11270,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>23-200</t>
+          <t>23-203</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -11344,7 +11344,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>28-275</t>
+          <t>28-278</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -11418,7 +11418,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>22-309</t>
+          <t>22-312</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -11492,7 +11492,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>18-179</t>
+          <t>18-182</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -11566,7 +11566,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>27-167</t>
+          <t>27-170</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -11640,7 +11640,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>18-003</t>
+          <t>18-006</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -11714,7 +11714,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>33-094</t>
+          <t>33-097</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -11786,7 +11786,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>27-355</t>
+          <t>27-358</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -11860,7 +11860,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>30-106</t>
+          <t>30-109</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -11932,7 +11932,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>25-037</t>
+          <t>25-040</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -11996,7 +11996,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>28-099</t>
+          <t>28-102</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -12068,7 +12068,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>27-292</t>
+          <t>27-295</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -12140,7 +12140,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>26-139</t>
+          <t>26-142</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -12212,7 +12212,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>25-104</t>
+          <t>25-107</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -12628,7 +12628,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>29-190</t>
+          <t>29-193</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -12720,7 +12720,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>24-000</t>
+          <t>24-003</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -12812,7 +12812,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>27-095</t>
+          <t>27-098</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -12904,7 +12904,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>23-280</t>
+          <t>23-283</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -12996,7 +12996,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>26-069</t>
+          <t>26-072</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -13088,7 +13088,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>31-284</t>
+          <t>31-287</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -13180,7 +13180,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>30-110</t>
+          <t>30-113</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -13272,7 +13272,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>25-286</t>
+          <t>25-289</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -13364,7 +13364,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>26-097</t>
+          <t>26-100</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -13456,7 +13456,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>23-279</t>
+          <t>23-282</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -13548,7 +13548,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>23-200</t>
+          <t>23-203</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -13640,7 +13640,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>28-275</t>
+          <t>28-278</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -13732,7 +13732,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>22-309</t>
+          <t>22-312</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -13824,7 +13824,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>18-179</t>
+          <t>18-182</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -13916,7 +13916,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>27-167</t>
+          <t>27-170</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -14008,7 +14008,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>18-003</t>
+          <t>18-006</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -14100,7 +14100,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>33-094</t>
+          <t>33-097</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -14192,7 +14192,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>27-355</t>
+          <t>27-358</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -14284,7 +14284,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>30-106</t>
+          <t>30-109</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -14376,7 +14376,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>25-037</t>
+          <t>25-040</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -14468,7 +14468,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>28-099</t>
+          <t>28-102</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -14560,7 +14560,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>27-292</t>
+          <t>27-295</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -14652,7 +14652,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>26-139</t>
+          <t>26-142</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -14744,7 +14744,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>25-104</t>
+          <t>25-107</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -15163,7 +15163,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>29-190</t>
+          <t>29-193</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -15231,7 +15231,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>24-000</t>
+          <t>24-003</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -15299,7 +15299,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>27-095</t>
+          <t>27-098</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -15367,7 +15367,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>23-280</t>
+          <t>23-283</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -15435,7 +15435,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>26-069</t>
+          <t>26-072</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -15503,7 +15503,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>31-284</t>
+          <t>31-287</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -15571,7 +15571,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>30-110</t>
+          <t>30-113</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -15639,7 +15639,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>25-286</t>
+          <t>25-289</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -15707,7 +15707,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>26-097</t>
+          <t>26-100</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -15775,7 +15775,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>23-279</t>
+          <t>23-282</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -15843,7 +15843,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>23-200</t>
+          <t>23-203</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -15911,7 +15911,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>28-275</t>
+          <t>28-278</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -15979,7 +15979,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>22-309</t>
+          <t>22-312</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -16047,7 +16047,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>18-179</t>
+          <t>18-182</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -16115,7 +16115,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>27-167</t>
+          <t>27-170</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -16183,7 +16183,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>18-003</t>
+          <t>18-006</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -16251,7 +16251,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>33-094</t>
+          <t>33-097</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -16319,7 +16319,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>27-355</t>
+          <t>27-358</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -16387,7 +16387,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>30-106</t>
+          <t>30-109</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -16455,7 +16455,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>25-037</t>
+          <t>25-040</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -16523,7 +16523,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>28-099</t>
+          <t>28-102</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -16591,7 +16591,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>27-292</t>
+          <t>27-295</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -16659,7 +16659,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>26-139</t>
+          <t>26-142</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -16727,7 +16727,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>25-104</t>
+          <t>25-107</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -17090,7 +17090,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>29-190</t>
+          <t>29-193</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -17161,7 +17161,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>24-000</t>
+          <t>24-003</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -17232,7 +17232,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>27-095</t>
+          <t>27-098</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -17303,7 +17303,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>23-280</t>
+          <t>23-283</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -17374,7 +17374,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>26-069</t>
+          <t>26-072</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -17445,7 +17445,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>31-284</t>
+          <t>31-287</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -17516,7 +17516,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>30-110</t>
+          <t>30-113</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -17587,7 +17587,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>25-286</t>
+          <t>25-289</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -17658,7 +17658,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>26-097</t>
+          <t>26-100</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -17729,7 +17729,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>23-279</t>
+          <t>23-282</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -17800,7 +17800,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>23-200</t>
+          <t>23-203</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -17871,7 +17871,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>28-275</t>
+          <t>28-278</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -17942,7 +17942,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>22-309</t>
+          <t>22-312</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -18013,7 +18013,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>18-179</t>
+          <t>18-182</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -18084,7 +18084,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>27-167</t>
+          <t>27-170</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -18155,7 +18155,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>18-003</t>
+          <t>18-006</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -18226,7 +18226,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>33-094</t>
+          <t>33-097</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -18297,7 +18297,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>27-355</t>
+          <t>27-358</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -18368,7 +18368,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>30-106</t>
+          <t>30-109</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -18439,7 +18439,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>25-037</t>
+          <t>25-040</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -18510,7 +18510,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>28-099</t>
+          <t>28-102</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -18581,7 +18581,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>27-292</t>
+          <t>27-295</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -18652,7 +18652,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>26-139</t>
+          <t>26-142</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -18723,7 +18723,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>25-104</t>
+          <t>25-107</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -19092,7 +19092,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>29-190</t>
+          <t>29-193</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -19163,7 +19163,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>24-000</t>
+          <t>24-003</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -19234,7 +19234,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>27-095</t>
+          <t>27-098</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -19305,7 +19305,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>23-280</t>
+          <t>23-283</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -19376,7 +19376,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>26-069</t>
+          <t>26-072</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -19447,7 +19447,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>31-284</t>
+          <t>31-287</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -19518,7 +19518,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>30-110</t>
+          <t>30-113</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -19589,7 +19589,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>25-286</t>
+          <t>25-289</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -19660,7 +19660,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>26-097</t>
+          <t>26-100</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -19731,7 +19731,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>23-279</t>
+          <t>23-282</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -19802,7 +19802,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>23-200</t>
+          <t>23-203</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -19873,7 +19873,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>28-275</t>
+          <t>28-278</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -19944,7 +19944,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>22-309</t>
+          <t>22-312</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -20015,7 +20015,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>18-179</t>
+          <t>18-182</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -20086,7 +20086,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>27-167</t>
+          <t>27-170</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -20157,7 +20157,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>18-003</t>
+          <t>18-006</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -20228,7 +20228,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>33-094</t>
+          <t>33-097</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -20299,7 +20299,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>27-355</t>
+          <t>27-358</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -20370,7 +20370,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>30-106</t>
+          <t>30-109</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -20441,7 +20441,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>25-037</t>
+          <t>25-040</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -20512,7 +20512,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>28-099</t>
+          <t>28-102</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -20583,7 +20583,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>27-292</t>
+          <t>27-295</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -20654,7 +20654,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>26-139</t>
+          <t>26-142</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -20723,7 +20723,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>25-104</t>
+          <t>25-107</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -21131,7 +21131,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>29-190</t>
+          <t>29-193</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -21220,7 +21220,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>24-000</t>
+          <t>24-003</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -21309,7 +21309,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>27-095</t>
+          <t>27-098</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -21398,7 +21398,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>23-280</t>
+          <t>23-283</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -21487,7 +21487,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>26-069</t>
+          <t>26-072</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -21576,7 +21576,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>31-284</t>
+          <t>31-287</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -21665,7 +21665,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>30-110</t>
+          <t>30-113</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -21754,7 +21754,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>25-286</t>
+          <t>25-289</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -21843,7 +21843,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>26-097</t>
+          <t>26-100</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -21932,7 +21932,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>23-279</t>
+          <t>23-282</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -22021,7 +22021,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>23-200</t>
+          <t>23-203</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -22110,7 +22110,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>28-275</t>
+          <t>28-278</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -22199,7 +22199,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>22-309</t>
+          <t>22-312</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -22288,7 +22288,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>18-179</t>
+          <t>18-182</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -22377,7 +22377,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>27-167</t>
+          <t>27-170</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -22466,7 +22466,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>18-003</t>
+          <t>18-006</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -22555,7 +22555,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>33-094</t>
+          <t>33-097</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -22644,7 +22644,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>27-355</t>
+          <t>27-358</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -22733,7 +22733,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>30-106</t>
+          <t>30-109</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -22822,7 +22822,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>25-037</t>
+          <t>25-040</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -22911,7 +22911,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>28-099</t>
+          <t>28-102</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -23000,7 +23000,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>27-292</t>
+          <t>27-295</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -23089,7 +23089,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>26-139</t>
+          <t>26-142</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -23174,7 +23174,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>25-104</t>
+          <t>25-107</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -23673,7 +23673,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>29-190</t>
+          <t>29-193</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -23780,7 +23780,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>24-000</t>
+          <t>24-003</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -23887,7 +23887,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>27-095</t>
+          <t>27-098</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -23994,7 +23994,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>23-280</t>
+          <t>23-283</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -24101,7 +24101,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>26-069</t>
+          <t>26-072</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -24208,7 +24208,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>31-284</t>
+          <t>31-287</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -24315,7 +24315,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>30-110</t>
+          <t>30-113</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -24422,7 +24422,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>25-286</t>
+          <t>25-289</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -24529,7 +24529,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>26-097</t>
+          <t>26-100</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -24636,7 +24636,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>23-279</t>
+          <t>23-282</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -24743,7 +24743,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>23-200</t>
+          <t>23-203</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -24850,7 +24850,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>28-275</t>
+          <t>28-278</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -24957,7 +24957,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>22-309</t>
+          <t>22-312</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -25064,7 +25064,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>18-179</t>
+          <t>18-182</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -25171,7 +25171,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>27-167</t>
+          <t>27-170</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -25278,7 +25278,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>18-003</t>
+          <t>18-006</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -25385,7 +25385,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>33-094</t>
+          <t>33-097</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -25492,7 +25492,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>27-355</t>
+          <t>27-358</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -25599,7 +25599,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>30-106</t>
+          <t>30-109</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -25706,7 +25706,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>25-037</t>
+          <t>25-040</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -25813,7 +25813,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>28-099</t>
+          <t>28-102</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -25920,7 +25920,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>27-292</t>
+          <t>27-295</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -26027,7 +26027,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>26-139</t>
+          <t>26-142</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -26134,7 +26134,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>25-104</t>
+          <t>25-107</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -26241,7 +26241,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>22-079</t>
+          <t>22-082</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -26294,7 +26294,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>18-183</t>
+          <t>18-186</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -26347,7 +26347,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>19-104</t>
+          <t>19-107</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -26400,7 +26400,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>19-171</t>
+          <t>19-174</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -26453,7 +26453,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>35-248</t>
+          <t>35-251</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -26506,7 +26506,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>18-241</t>
+          <t>18-244</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -26559,7 +26559,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>25-298</t>
+          <t>25-301</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -26612,7 +26612,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>21-216</t>
+          <t>21-219</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -26665,7 +26665,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>16-252</t>
+          <t>16-255</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -26718,7 +26718,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>26-314</t>
+          <t>26-317</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -26771,7 +26771,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>19-011</t>
+          <t>19-014</t>
         </is>
       </c>
       <c r="E38" t="n">

</xml_diff>